<commit_message>
Removed impossible combination of pointer to reference and whitelisted for coverage unreachable (but necessary) virtual functions
</commit_message>
<xml_diff>
--- a/test/Function_Mock_CPP/CppUGenMock UTs.xlsx
+++ b/test/Function_Mock_CPP/CppUGenMock UTs.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\CppUMockGen\test\Function_CPP\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12000" windowHeight="5100" activeTab="1"/>
   </bookViews>
@@ -15,7 +10,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1569" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1593" uniqueCount="225">
   <si>
     <t>VoidReturnNoParameters</t>
   </si>
@@ -705,7 +700,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1229,7 +1224,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1243,7 +1238,7 @@
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.85546875" customWidth="1"/>
     <col min="2" max="2" width="67.85546875" bestFit="1" customWidth="1"/>
@@ -1536,13 +1531,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:M186"/>
+  <dimension ref="B2:M190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A137" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K157" sqref="K157"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J152" sqref="J152"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.5703125" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
@@ -5826,439 +5821,391 @@
       <c r="M146" s="36"/>
     </row>
     <row r="147" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B147" s="34" t="s">
+      <c r="B147" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="C147" s="34" t="s">
+      <c r="C147" s="36"/>
+      <c r="D147" s="36" t="s">
+        <v>104</v>
+      </c>
+      <c r="E147" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="F147" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="G147" s="36"/>
+      <c r="H147" s="36"/>
+      <c r="I147" s="36"/>
+      <c r="J147" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="K147" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="L147" s="37"/>
+      <c r="M147" s="36"/>
+    </row>
+    <row r="148" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B148" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="D147" s="34" t="s">
-        <v>58</v>
-      </c>
-      <c r="E147" s="34" t="s">
-        <v>55</v>
-      </c>
-      <c r="F147" s="34" t="s">
+      <c r="C148" s="36"/>
+      <c r="D148" s="36" t="s">
+        <v>104</v>
+      </c>
+      <c r="E148" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="F148" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="G148" s="36"/>
+      <c r="H148" s="36"/>
+      <c r="I148" s="36"/>
+      <c r="J148" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="K148" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="L148" s="37"/>
+      <c r="M148" s="36"/>
+    </row>
+    <row r="149" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B149" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="C149" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="D149" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="E149" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="F149" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="G147" s="34"/>
-      <c r="H147" s="34"/>
-      <c r="I147" s="34"/>
-      <c r="J147" s="34" t="s">
+      <c r="G149" s="34"/>
+      <c r="H149" s="34"/>
+      <c r="I149" s="34"/>
+      <c r="J149" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="K147" s="34" t="s">
+      <c r="K149" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="L147" s="35" t="s">
+      <c r="L149" s="35" t="s">
         <v>146</v>
       </c>
-      <c r="M147" s="34" t="s">
+      <c r="M149" s="34" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="148" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B148" s="34" t="s">
+    <row r="150" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B150" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="C148" s="34" t="s">
+      <c r="C150" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="D148" s="34" t="s">
-        <v>58</v>
-      </c>
-      <c r="E148" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="F148" s="34" t="s">
+      <c r="D150" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="E150" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="F150" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="G148" s="34"/>
-      <c r="H148" s="34"/>
-      <c r="I148" s="34"/>
-      <c r="J148" s="34" t="s">
+      <c r="G150" s="34"/>
+      <c r="H150" s="34"/>
+      <c r="I150" s="34"/>
+      <c r="J150" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="K148" s="34" t="s">
+      <c r="K150" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="L148" s="35" t="s">
+      <c r="L150" s="35" t="s">
         <v>148</v>
       </c>
-      <c r="M148" s="34" t="s">
+      <c r="M150" s="34" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="149" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B149" s="36" t="s">
+    <row r="151" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B151" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="C149" s="36"/>
-      <c r="D149" s="36" t="s">
+      <c r="C151" s="36"/>
+      <c r="D151" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="E149" s="36" t="s">
-        <v>55</v>
-      </c>
-      <c r="F149" s="36" t="s">
+      <c r="E151" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="F151" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="G149" s="36"/>
-      <c r="H149" s="36"/>
-      <c r="I149" s="36"/>
-      <c r="J149" s="36" t="s">
+      <c r="G151" s="36"/>
+      <c r="H151" s="36"/>
+      <c r="I151" s="36"/>
+      <c r="J151" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="K149" s="36" t="s">
+      <c r="K151" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="L149" s="37"/>
-      <c r="M149" s="36"/>
-    </row>
-    <row r="150" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B150" s="38" t="s">
+      <c r="L151" s="37"/>
+      <c r="M151" s="36"/>
+    </row>
+    <row r="152" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B152" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="C150" s="38"/>
-      <c r="D150" s="38" t="s">
+      <c r="C152" s="38"/>
+      <c r="D152" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="E150" s="38" t="s">
-        <v>56</v>
-      </c>
-      <c r="F150" s="38" t="s">
+      <c r="E152" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="F152" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="G150" s="38"/>
-      <c r="H150" s="38"/>
-      <c r="I150" s="38"/>
-      <c r="J150" s="38" t="s">
+      <c r="G152" s="38"/>
+      <c r="H152" s="38"/>
+      <c r="I152" s="38"/>
+      <c r="J152" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="K150" s="38" t="s">
+      <c r="K152" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="L150" s="39"/>
-      <c r="M150" s="38"/>
-    </row>
-    <row r="151" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B151" s="20" t="s">
+      <c r="L152" s="39"/>
+      <c r="M152" s="38"/>
+    </row>
+    <row r="153" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B153" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="C153" s="36"/>
+      <c r="D153" s="36" t="s">
+        <v>104</v>
+      </c>
+      <c r="E153" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="F153" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="G153" s="36"/>
+      <c r="H153" s="36"/>
+      <c r="I153" s="36"/>
+      <c r="J153" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="K153" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="L153" s="37"/>
+      <c r="M153" s="36"/>
+    </row>
+    <row r="154" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B154" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C154" s="38"/>
+      <c r="D154" s="38" t="s">
+        <v>104</v>
+      </c>
+      <c r="E154" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="F154" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="G154" s="38"/>
+      <c r="H154" s="38"/>
+      <c r="I154" s="38"/>
+      <c r="J154" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="K154" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="L154" s="39"/>
+      <c r="M154" s="38"/>
+    </row>
+    <row r="155" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B155" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="C151" s="20" t="s">
+      <c r="C155" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="D151" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="E151" s="20"/>
-      <c r="F151" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="G151" s="20"/>
-      <c r="H151" s="20"/>
-      <c r="I151" s="20"/>
-      <c r="J151" s="20" t="s">
+      <c r="D155" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="E155" s="20"/>
+      <c r="F155" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="G155" s="20"/>
+      <c r="H155" s="20"/>
+      <c r="I155" s="20"/>
+      <c r="J155" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="K151" s="20" t="s">
+      <c r="K155" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="L151" s="20" t="s">
+      <c r="L155" s="20" t="s">
         <v>211</v>
       </c>
-      <c r="M151" s="20" t="s">
+      <c r="M155" s="20" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="152" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B152" s="14" t="s">
+    <row r="156" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B156" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="C152" s="14" t="s">
+      <c r="C156" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="D152" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="E152" s="14"/>
-      <c r="F152" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="G152" s="14"/>
-      <c r="H152" s="14"/>
-      <c r="I152" s="14"/>
-      <c r="J152" s="14" t="s">
+      <c r="D156" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E156" s="14"/>
+      <c r="F156" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="G156" s="14"/>
+      <c r="H156" s="14"/>
+      <c r="I156" s="14"/>
+      <c r="J156" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="K152" s="14" t="s">
+      <c r="K156" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="L152" s="14"/>
-      <c r="M152" s="14"/>
-    </row>
-    <row r="153" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B153" s="14" t="s">
+      <c r="L156" s="14"/>
+      <c r="M156" s="14"/>
+    </row>
+    <row r="157" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B157" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="C153" s="14" t="s">
+      <c r="C157" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="D153" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="E153" s="14"/>
-      <c r="F153" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="G153" s="14"/>
-      <c r="H153" s="14"/>
-      <c r="I153" s="14"/>
-      <c r="J153" s="14" t="s">
+      <c r="D157" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E157" s="14"/>
+      <c r="F157" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="G157" s="14"/>
+      <c r="H157" s="14"/>
+      <c r="I157" s="14"/>
+      <c r="J157" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="K153" s="14" t="s">
+      <c r="K157" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="L153" s="14"/>
-      <c r="M153" s="14"/>
-    </row>
-    <row r="154" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B154" s="14" t="s">
+      <c r="L157" s="14"/>
+      <c r="M157" s="14"/>
+    </row>
+    <row r="158" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B158" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="C154" s="14" t="s">
+      <c r="C158" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="D154" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="E154" s="14"/>
-      <c r="F154" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="G154" s="14"/>
-      <c r="H154" s="14"/>
-      <c r="I154" s="14"/>
-      <c r="J154" s="14" t="s">
+      <c r="D158" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E158" s="14"/>
+      <c r="F158" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="G158" s="14"/>
+      <c r="H158" s="14"/>
+      <c r="I158" s="14"/>
+      <c r="J158" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="K154" s="14" t="s">
+      <c r="K158" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="L154" s="14"/>
-      <c r="M154" s="14"/>
-    </row>
-    <row r="155" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B155" s="14" t="s">
+      <c r="L158" s="14"/>
+      <c r="M158" s="14"/>
+    </row>
+    <row r="159" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B159" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="C155" s="14" t="s">
+      <c r="C159" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="D155" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="E155" s="14"/>
-      <c r="F155" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="G155" s="14"/>
-      <c r="H155" s="14"/>
-      <c r="I155" s="14"/>
-      <c r="J155" s="14" t="s">
+      <c r="D159" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E159" s="14"/>
+      <c r="F159" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="G159" s="14"/>
+      <c r="H159" s="14"/>
+      <c r="I159" s="14"/>
+      <c r="J159" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="K155" s="14" t="s">
+      <c r="K159" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="L155" s="14"/>
-      <c r="M155" s="14"/>
-    </row>
-    <row r="156" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B156" s="15" t="s">
+      <c r="L159" s="14"/>
+      <c r="M159" s="14"/>
+    </row>
+    <row r="160" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B160" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="C156" s="15" t="s">
+      <c r="C160" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="D156" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="E156" s="15"/>
-      <c r="F156" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="G156" s="15"/>
-      <c r="H156" s="15"/>
-      <c r="I156" s="15"/>
-      <c r="J156" s="15" t="s">
+      <c r="D160" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E160" s="15"/>
+      <c r="F160" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="G160" s="15"/>
+      <c r="H160" s="15"/>
+      <c r="I160" s="15"/>
+      <c r="J160" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="K156" s="15" t="s">
+      <c r="K160" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="L156" s="15"/>
-      <c r="M156" s="15"/>
-    </row>
-    <row r="157" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B157" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="C157" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="D157" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="E157" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="F157" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="G157" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="H157" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="I157" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="J157" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="K157" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="L157" s="41" t="s">
-        <v>202</v>
-      </c>
-      <c r="M157" s="41" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="158" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B158" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="C158" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="D158" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="E158" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="F158" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="G158" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="H158" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="I158" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="J158" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="K158" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="L158" s="41" t="s">
-        <v>203</v>
-      </c>
-      <c r="M158" s="41" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="159" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B159" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="C159" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="D159" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="E159" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="F159" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="G159" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="H159" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="I159" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="J159" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="K159" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="L159" s="41" t="s">
-        <v>204</v>
-      </c>
-      <c r="M159" s="41" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="160" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B160" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="C160" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="D160" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="E160" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="F160" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="G160" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="H160" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="I160" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="J160" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="K160" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="L160" s="41" t="s">
-        <v>205</v>
-      </c>
-      <c r="M160" s="41" t="s">
-        <v>222</v>
-      </c>
+      <c r="L160" s="15"/>
+      <c r="M160" s="15"/>
     </row>
     <row r="161" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B161" s="12" t="s">
         <v>77</v>
       </c>
       <c r="C161" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D161" s="12" t="s">
         <v>58</v>
@@ -6270,7 +6217,7 @@
         <v>52</v>
       </c>
       <c r="G161" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H161" s="12" t="s">
         <v>52</v>
@@ -6279,16 +6226,16 @@
         <v>55</v>
       </c>
       <c r="J161" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K161" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L161" s="41" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="M161" s="41" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="162" spans="2:13" x14ac:dyDescent="0.25">
@@ -6296,7 +6243,7 @@
         <v>77</v>
       </c>
       <c r="C162" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D162" s="12" t="s">
         <v>58</v>
@@ -6308,30 +6255,30 @@
         <v>52</v>
       </c>
       <c r="G162" s="12" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H162" s="12" t="s">
         <v>52</v>
       </c>
       <c r="I162" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J162" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K162" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L162" s="41" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="M162" s="41" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="163" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B163" s="12" t="s">
-        <v>35</v>
+        <v>77</v>
       </c>
       <c r="C163" s="12" t="s">
         <v>55</v>
@@ -6352,7 +6299,7 @@
         <v>52</v>
       </c>
       <c r="I163" s="12" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J163" s="12" t="s">
         <v>61</v>
@@ -6360,19 +6307,19 @@
       <c r="K163" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="L163" s="12" t="s">
-        <v>202</v>
-      </c>
-      <c r="M163" s="12" t="s">
-        <v>219</v>
+      <c r="L163" s="41" t="s">
+        <v>204</v>
+      </c>
+      <c r="M163" s="41" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="164" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B164" s="12" t="s">
-        <v>35</v>
+        <v>77</v>
       </c>
       <c r="C164" s="12" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D164" s="12" t="s">
         <v>58</v>
@@ -6384,7 +6331,7 @@
         <v>52</v>
       </c>
       <c r="G164" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H164" s="12" t="s">
         <v>52</v>
@@ -6393,24 +6340,24 @@
         <v>55</v>
       </c>
       <c r="J164" s="12" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="K164" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="L164" s="12" t="s">
-        <v>203</v>
-      </c>
-      <c r="M164" s="12" t="s">
-        <v>220</v>
+        <v>62</v>
+      </c>
+      <c r="L164" s="41" t="s">
+        <v>205</v>
+      </c>
+      <c r="M164" s="41" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="165" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B165" s="12" t="s">
-        <v>35</v>
+        <v>77</v>
       </c>
       <c r="C165" s="12" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D165" s="12" t="s">
         <v>58</v>
@@ -6422,30 +6369,30 @@
         <v>52</v>
       </c>
       <c r="G165" s="12" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H165" s="12" t="s">
         <v>52</v>
       </c>
       <c r="I165" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J165" s="12" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="K165" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="L165" s="12" t="s">
-        <v>204</v>
-      </c>
-      <c r="M165" s="12" t="s">
-        <v>221</v>
+        <v>62</v>
+      </c>
+      <c r="L165" s="41" t="s">
+        <v>206</v>
+      </c>
+      <c r="M165" s="41" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="166" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B166" s="12" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="C166" s="12" t="s">
         <v>56</v>
@@ -6466,7 +6413,7 @@
         <v>52</v>
       </c>
       <c r="I166" s="12" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J166" s="12" t="s">
         <v>62</v>
@@ -6474,19 +6421,19 @@
       <c r="K166" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="L166" s="12" t="s">
-        <v>205</v>
-      </c>
-      <c r="M166" s="12" t="s">
-        <v>222</v>
+      <c r="L166" s="41" t="s">
+        <v>207</v>
+      </c>
+      <c r="M166" s="41" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="167" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B167" s="12" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="C167" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D167" s="12" t="s">
         <v>58</v>
@@ -6498,7 +6445,7 @@
         <v>52</v>
       </c>
       <c r="G167" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H167" s="12" t="s">
         <v>52</v>
@@ -6507,304 +6454,328 @@
         <v>55</v>
       </c>
       <c r="J167" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K167" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L167" s="12" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="M167" s="12" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="168" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B168" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C168" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D168" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E168" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F168" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="G168" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="H168" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="I168" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="J168" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="K168" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="L168" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="M168" s="12" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="169" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B169" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C169" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D169" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E169" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F169" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="G169" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="H169" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="I169" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="J169" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="K169" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="L169" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="M169" s="12" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="170" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B170" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="C168" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="D168" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="E168" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="F168" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="G168" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="H168" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="I168" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="J168" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="K168" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="L168" s="12" t="s">
+      <c r="C170" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D170" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E170" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F170" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="G170" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="H170" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="I170" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="J170" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="K170" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="L170" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="M170" s="12" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="171" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B171" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C171" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D171" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E171" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F171" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="G171" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="H171" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="I171" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="J171" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="K171" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="L171" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="M171" s="12" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="172" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B172" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C172" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D172" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E172" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F172" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="G172" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="H172" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="I172" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="J172" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="K172" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="L172" s="12" t="s">
         <v>207</v>
       </c>
-      <c r="M168" s="12" t="s">
+      <c r="M172" s="12" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="169" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B169" s="8" t="s">
+    <row r="173" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B173" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="C169" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="D169" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="E169" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="F169" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="G169" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="H169" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="I169" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="J169" s="8" t="s">
+      <c r="C173" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D173" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E173" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F173" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G173" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="H173" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="I173" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="J173" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="K169" s="8" t="s">
+      <c r="K173" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="L169" s="8" t="s">
+      <c r="L173" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="M169" s="8" t="s">
+      <c r="M173" s="8" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="170" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B170" s="8" t="s">
+    <row r="174" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B174" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="C170" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="D170" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="E170" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="F170" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="G170" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="H170" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="I170" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="J170" s="8" t="s">
+      <c r="C174" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D174" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E174" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F174" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G174" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="H174" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="I174" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="J174" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="K170" s="8" t="s">
+      <c r="K174" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="L170" s="8" t="s">
+      <c r="L174" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="M170" s="8" t="s">
+      <c r="M174" s="8" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="171" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B171" s="8" t="s">
+    <row r="175" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B175" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="C171" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="D171" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="E171" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="F171" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="G171" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="H171" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="I171" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="J171" s="8" t="s">
+      <c r="C175" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D175" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E175" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F175" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G175" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="H175" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="I175" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="J175" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="K171" s="8" t="s">
+      <c r="K175" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="L171" s="8" t="s">
+      <c r="L175" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="M171" s="8" t="s">
+      <c r="M175" s="8" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="172" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B172" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="C172" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="D172" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="E172" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="F172" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="G172" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="H172" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="I172" s="27"/>
-      <c r="J172" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="K172" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="L172" s="12"/>
-      <c r="M172" s="12"/>
-    </row>
-    <row r="173" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B173" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="C173" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="D173" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="E173" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="F173" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="G173" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="H173" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="I173" s="27"/>
-      <c r="J173" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="K173" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="L173" s="12"/>
-      <c r="M173" s="12"/>
-    </row>
-    <row r="174" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B174" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="C174" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="D174" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="E174" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="F174" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="G174" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="H174" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="I174" s="27"/>
-      <c r="J174" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="K174" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="L174" s="12"/>
-      <c r="M174" s="12"/>
-    </row>
-    <row r="175" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B175" s="27" t="s">
-        <v>80</v>
-      </c>
-      <c r="C175" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="D175" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="E175" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="F175" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="G175" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="H175" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="I175" s="27"/>
-      <c r="J175" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="K175" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="L175" s="12"/>
-      <c r="M175" s="12"/>
     </row>
     <row r="176" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B176" s="27" t="s">
-        <v>80</v>
+        <v>36</v>
       </c>
       <c r="C176" s="27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D176" s="27" t="s">
         <v>58</v>
@@ -6823,20 +6794,20 @@
       </c>
       <c r="I176" s="27"/>
       <c r="J176" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K176" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L176" s="12"/>
       <c r="M176" s="12"/>
     </row>
     <row r="177" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B177" s="27" t="s">
-        <v>80</v>
+        <v>36</v>
       </c>
       <c r="C177" s="27" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D177" s="27" t="s">
         <v>58</v>
@@ -6848,7 +6819,7 @@
         <v>52</v>
       </c>
       <c r="G177" s="27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H177" s="27" t="s">
         <v>52</v>
@@ -6865,7 +6836,7 @@
     </row>
     <row r="178" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B178" s="27" t="s">
-        <v>75</v>
+        <v>36</v>
       </c>
       <c r="C178" s="27" t="s">
         <v>55</v>
@@ -6880,27 +6851,27 @@
         <v>52</v>
       </c>
       <c r="G178" s="27" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H178" s="27" t="s">
         <v>52</v>
       </c>
       <c r="I178" s="27"/>
       <c r="J178" s="27" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="K178" s="27" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L178" s="12"/>
       <c r="M178" s="12"/>
     </row>
     <row r="179" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B179" s="27" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="C179" s="27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D179" s="27" t="s">
         <v>58</v>
@@ -6919,20 +6890,20 @@
       </c>
       <c r="I179" s="27"/>
       <c r="J179" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K179" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L179" s="12"/>
       <c r="M179" s="12"/>
     </row>
     <row r="180" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B180" s="27" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="C180" s="27" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D180" s="27" t="s">
         <v>58</v>
@@ -6944,7 +6915,7 @@
         <v>52</v>
       </c>
       <c r="G180" s="27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H180" s="27" t="s">
         <v>52</v>
@@ -6961,7 +6932,7 @@
     </row>
     <row r="181" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B181" s="27" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="C181" s="27" t="s">
         <v>55</v>
@@ -6976,27 +6947,27 @@
         <v>52</v>
       </c>
       <c r="G181" s="27" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H181" s="27" t="s">
         <v>52</v>
       </c>
       <c r="I181" s="27"/>
       <c r="J181" s="27" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="K181" s="27" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L181" s="12"/>
       <c r="M181" s="12"/>
     </row>
     <row r="182" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B182" s="27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C182" s="27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D182" s="27" t="s">
         <v>58</v>
@@ -7015,20 +6986,20 @@
       </c>
       <c r="I182" s="27"/>
       <c r="J182" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K182" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L182" s="12"/>
       <c r="M182" s="12"/>
     </row>
     <row r="183" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B183" s="27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C183" s="27" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D183" s="27" t="s">
         <v>58</v>
@@ -7040,7 +7011,7 @@
         <v>52</v>
       </c>
       <c r="G183" s="27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H183" s="27" t="s">
         <v>52</v>
@@ -7057,7 +7028,7 @@
     </row>
     <row r="184" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B184" s="27" t="s">
-        <v>129</v>
+        <v>75</v>
       </c>
       <c r="C184" s="27" t="s">
         <v>55</v>
@@ -7072,27 +7043,27 @@
         <v>52</v>
       </c>
       <c r="G184" s="27" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H184" s="27" t="s">
         <v>52</v>
       </c>
       <c r="I184" s="27"/>
       <c r="J184" s="27" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="K184" s="27" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L184" s="12"/>
       <c r="M184" s="12"/>
     </row>
     <row r="185" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B185" s="27" t="s">
-        <v>129</v>
+        <v>76</v>
       </c>
       <c r="C185" s="27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D185" s="27" t="s">
         <v>58</v>
@@ -7111,45 +7082,173 @@
       </c>
       <c r="I185" s="27"/>
       <c r="J185" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K185" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L185" s="12"/>
       <c r="M185" s="12"/>
     </row>
     <row r="186" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B186" s="28" t="s">
+      <c r="B186" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="C186" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="D186" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="E186" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="F186" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="G186" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="H186" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="I186" s="27"/>
+      <c r="J186" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="K186" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="L186" s="12"/>
+      <c r="M186" s="12"/>
+    </row>
+    <row r="187" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B187" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="C187" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="D187" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="E187" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="F187" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="G187" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="H187" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="I187" s="27"/>
+      <c r="J187" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="K187" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="L187" s="12"/>
+      <c r="M187" s="12"/>
+    </row>
+    <row r="188" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B188" s="27" t="s">
         <v>129</v>
       </c>
-      <c r="C186" s="28" t="s">
-        <v>55</v>
-      </c>
-      <c r="D186" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="E186" s="28" t="s">
-        <v>55</v>
-      </c>
-      <c r="F186" s="28" t="s">
-        <v>52</v>
-      </c>
-      <c r="G186" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="H186" s="28" t="s">
-        <v>52</v>
-      </c>
-      <c r="I186" s="28"/>
-      <c r="J186" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="K186" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="L186" s="19"/>
-      <c r="M186" s="19"/>
+      <c r="C188" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="D188" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="E188" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="F188" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="G188" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="H188" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="I188" s="27"/>
+      <c r="J188" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="K188" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="L188" s="12"/>
+      <c r="M188" s="12"/>
+    </row>
+    <row r="189" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B189" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="C189" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="D189" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="E189" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="F189" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="G189" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="H189" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="I189" s="27"/>
+      <c r="J189" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="K189" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="L189" s="12"/>
+      <c r="M189" s="12"/>
+    </row>
+    <row r="190" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B190" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="C190" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="D190" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="E190" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="F190" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="G190" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="H190" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="I190" s="28"/>
+      <c r="J190" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="K190" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="L190" s="19"/>
+      <c r="M190" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>